<commit_message>
Atualização automática de CANOAS.xlsx
</commit_message>
<xml_diff>
--- a/CANOAS.xlsx
+++ b/CANOAS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{59BA5CB8-1E58-4C9D-9424-F1835CFD9EC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1120E5F7-D5D3-4628-8071-3A17CD9E5790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,20 +23,7 @@
     <sheet name="Recolhimento x Eliminacao" sheetId="7" r:id="rId8"/>
     <sheet name="Desarquivamentos Pendentes" sheetId="8" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -1155,7 +1142,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1216,30 +1203,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -1257,7 +1220,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1296,17 +1259,12 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1353,7 +1311,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{6E6EB897-0DFC-4CBF-9823-812AEFD25BD9}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{85D03003-7749-4BD2-B0C1-21DF9ACCD378}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1383,10 +1341,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A820CF1B-2FE9-4625-B5E6-99CE5CF03D71}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CF265E7-36F1-43D8-837A-0A9A43A62B7B}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1424,7 +1382,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0AB003E-2A03-4DA4-AA28-C8985DFA0C67}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44156AED-8472-4F6D-82F7-C047D8A1E12C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1487,7 +1445,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C0611E9-4214-49D2-AEF0-FF16207C6C1C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57AA166A-814F-496D-A83E-4B3DE66B8A90}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1506,7 +1464,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4AD81A9-1508-F057-F1A1-05A23897679F}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA1D7217-3408-68E5-9704-68F28D9DA570}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1555,7 +1513,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E32339F-3ECA-2CEC-51F4-5D9B0BC13BF4}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1415A990-5B6A-171B-C0CC-B257067A3C98}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1574,7 +1532,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6F2CDDE-49D3-F741-BA58-CB0CD732509D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D800DEA0-246C-D577-492B-E16D657133A9}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1605,7 +1563,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DAF5260-124D-5480-FEE6-3892F97B5039}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C59F2E16-1D7F-BF1F-FE2E-C23213359617}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1636,7 +1594,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C71B9E0-B09C-71E7-1019-D8727264A3BD}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA6ECF90-6497-F7D3-6125-921118132CE1}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1679,7 +1637,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51387386-F51A-4A52-B55B-168AFFDF5562}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8A031A0-C9F7-4A35-B6F7-3CC24DFF223E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1717,7 +1675,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5416AB8A-C5C5-43D2-AC8D-2F61EB41B2C3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{038EED0B-88D7-4A0F-B32F-94177BA6CCEC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1760,7 +1718,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF7E46D5-CEC3-4C4F-B56B-329E4CFB8D43}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{569288A8-6524-4553-931C-F22050EB4DC3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2073,7 +2031,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5407098-2ABA-4DD1-81AE-41434B5CF632}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E80246B-35E8-4F51-A561-447969C3BB08}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -2085,98 +2043,98 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="12.5703125" style="41"/>
-    <col min="6" max="6" width="2" style="41" customWidth="1"/>
-    <col min="7" max="16" width="13.42578125" style="41" customWidth="1"/>
-    <col min="17" max="16384" width="12.5703125" style="41"/>
+    <col min="1" max="5" width="12.5703125" style="38"/>
+    <col min="6" max="6" width="2" style="38" customWidth="1"/>
+    <col min="7" max="16" width="13.42578125" style="38" customWidth="1"/>
+    <col min="17" max="16384" width="12.5703125" style="38"/>
   </cols>
   <sheetData>
     <row r="1" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F1" s="40"/>
+      <c r="F1" s="37"/>
     </row>
     <row r="2" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F2" s="40"/>
+      <c r="F2" s="37"/>
     </row>
     <row r="3" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F3" s="40"/>
+      <c r="F3" s="37"/>
     </row>
     <row r="4" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F4" s="40"/>
+      <c r="F4" s="37"/>
     </row>
     <row r="5" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F5" s="40"/>
+      <c r="F5" s="37"/>
     </row>
     <row r="6" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F6" s="40"/>
+      <c r="F6" s="37"/>
     </row>
     <row r="7" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F7" s="40"/>
+      <c r="F7" s="37"/>
     </row>
     <row r="8" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F8" s="40"/>
+      <c r="F8" s="37"/>
     </row>
     <row r="9" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F9" s="40"/>
+      <c r="F9" s="37"/>
     </row>
     <row r="10" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F10" s="40"/>
+      <c r="F10" s="37"/>
     </row>
     <row r="11" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F11" s="40"/>
+      <c r="F11" s="37"/>
     </row>
     <row r="12" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F12" s="40"/>
+      <c r="F12" s="37"/>
     </row>
     <row r="13" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F13" s="40"/>
+      <c r="F13" s="37"/>
     </row>
     <row r="14" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F14" s="40"/>
+      <c r="F14" s="37"/>
     </row>
     <row r="15" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F15" s="40"/>
+      <c r="F15" s="37"/>
     </row>
     <row r="16" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F16" s="40"/>
+      <c r="F16" s="37"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F17" s="40"/>
+      <c r="F17" s="37"/>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F18" s="40"/>
+      <c r="F18" s="37"/>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F19" s="40"/>
+      <c r="F19" s="37"/>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F20" s="40"/>
+      <c r="F20" s="37"/>
     </row>
     <row r="21" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F21" s="40"/>
+      <c r="F21" s="37"/>
     </row>
     <row r="22" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F22" s="40"/>
+      <c r="F22" s="37"/>
     </row>
     <row r="23" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F23" s="40"/>
+      <c r="F23" s="37"/>
     </row>
     <row r="24" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F24" s="40"/>
+      <c r="F24" s="37"/>
     </row>
     <row r="25" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F25" s="40"/>
+      <c r="F25" s="37"/>
     </row>
     <row r="26" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F26" s="40"/>
+      <c r="F26" s="37"/>
     </row>
     <row r="27" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F27" s="40"/>
+      <c r="F27" s="37"/>
     </row>
     <row r="28" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F28" s="40"/>
+      <c r="F28" s="37"/>
     </row>
     <row r="29" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F29" s="40"/>
+      <c r="F29" s="37"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5442,19 +5400,19 @@
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="2" t="s">
         <v>273</v>
       </c>
     </row>
@@ -5488,46 +5446,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="18" t="s">
         <v>274</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="17" t="s">
         <v>275</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="17" t="s">
         <v>276</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="17" t="s">
         <v>277</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="17" t="s">
         <v>278</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="20" t="s">
+      <c r="J1" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="K1" s="20" t="s">
+      <c r="K1" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="L1" s="20" t="s">
+      <c r="L1" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="M1" s="20" t="s">
+      <c r="M1" s="17" t="s">
         <v>283</v>
       </c>
-      <c r="N1" s="20" t="s">
+      <c r="N1" s="17" t="s">
         <v>284</v>
       </c>
     </row>
@@ -5535,7 +5493,7 @@
       <c r="A2" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="B2" s="22">
+      <c r="B2" s="19">
         <v>453562</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -5547,10 +5505,10 @@
       <c r="E2" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="F2" s="23">
+      <c r="F2" s="20">
         <v>2888</v>
       </c>
-      <c r="G2" s="23">
+      <c r="G2" s="20">
         <v>3800</v>
       </c>
       <c r="H2" s="2" t="s">
@@ -5579,7 +5537,7 @@
       <c r="A3" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="B3" s="22">
+      <c r="B3" s="19">
         <v>453563</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -5591,10 +5549,10 @@
       <c r="E3" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="F3" s="23">
+      <c r="F3" s="20">
         <v>912</v>
       </c>
-      <c r="G3" s="23">
+      <c r="G3" s="20">
         <v>1200</v>
       </c>
       <c r="H3" s="2" t="s">
@@ -5623,7 +5581,7 @@
       <c r="A4" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="B4" s="22">
+      <c r="B4" s="19">
         <v>453564</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -5635,10 +5593,10 @@
       <c r="E4" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="F4" s="23">
+      <c r="F4" s="20">
         <v>912</v>
       </c>
-      <c r="G4" s="23">
+      <c r="G4" s="20">
         <v>1200</v>
       </c>
       <c r="H4" s="2" t="s">
@@ -5667,7 +5625,7 @@
       <c r="A5" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="B5" s="22">
+      <c r="B5" s="19">
         <v>453565</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -5679,10 +5637,10 @@
       <c r="E5" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="F5" s="23">
+      <c r="F5" s="20">
         <v>912</v>
       </c>
-      <c r="G5" s="23">
+      <c r="G5" s="20">
         <v>1200</v>
       </c>
       <c r="H5" s="2" t="s">
@@ -5711,7 +5669,7 @@
       <c r="A6" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="B6" s="22">
+      <c r="B6" s="19">
         <v>453566</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -5723,10 +5681,10 @@
       <c r="E6" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="F6" s="23">
+      <c r="F6" s="20">
         <v>912</v>
       </c>
-      <c r="G6" s="23">
+      <c r="G6" s="20">
         <v>1200</v>
       </c>
       <c r="H6" s="2" t="s">
@@ -5755,7 +5713,7 @@
       <c r="A7" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="B7" s="22">
+      <c r="B7" s="19">
         <v>453567</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -5767,10 +5725,10 @@
       <c r="E7" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="F7" s="23">
+      <c r="F7" s="20">
         <v>570.16</v>
       </c>
-      <c r="G7" s="23">
+      <c r="G7" s="20">
         <v>750</v>
       </c>
       <c r="H7" s="2" t="s">
@@ -5799,7 +5757,7 @@
       <c r="A8" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="B8" s="22">
+      <c r="B8" s="19">
         <v>453568</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -5811,10 +5769,10 @@
       <c r="E8" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="F8" s="23">
+      <c r="F8" s="20">
         <v>570.16</v>
       </c>
-      <c r="G8" s="23">
+      <c r="G8" s="20">
         <v>750</v>
       </c>
       <c r="H8" s="2" t="s">
@@ -5843,7 +5801,7 @@
       <c r="A9" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="B9" s="22">
+      <c r="B9" s="19">
         <v>453569</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -5855,10 +5813,10 @@
       <c r="E9" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="F9" s="23">
+      <c r="F9" s="20">
         <v>570.16</v>
       </c>
-      <c r="G9" s="23">
+      <c r="G9" s="20">
         <v>750</v>
       </c>
       <c r="H9" s="2" t="s">
@@ -5897,14 +5855,14 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.42578125" customWidth="1"/>
-    <col min="2" max="2" width="69.5703125" customWidth="1"/>
+    <col min="2" max="2" width="74.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="17" t="s">
         <v>298</v>
       </c>
     </row>
@@ -5935,79 +5893,79 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="22" t="s">
         <v>299</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="21" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="23" t="s">
         <v>301</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="23" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="23" t="s">
         <v>303</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="23" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="23" t="s">
         <v>305</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="23" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="23" t="s">
         <v>306</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="23" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="23" t="s">
         <v>307</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="23" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="23" t="s">
         <v>308</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="23" t="s">
         <v>302</v>
       </c>
     </row>
@@ -6032,54 +5990,55 @@
     <col min="6" max="6" width="12.5703125" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="14" width="13" customWidth="1"/>
-    <col min="15" max="15" width="30.85546875" customWidth="1"/>
+    <col min="9" max="12" width="13" customWidth="1"/>
+    <col min="13" max="13" width="42.140625" customWidth="1"/>
+    <col min="14" max="15" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="24" t="s">
         <v>309</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="25" t="s">
         <v>310</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="25" t="s">
         <v>311</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="25" t="s">
         <v>312</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="25" t="s">
         <v>313</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="26" t="s">
         <v>314</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="G1" s="26" t="s">
         <v>315</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="H1" s="24" t="s">
         <v>316</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="I1" s="24" t="s">
         <v>317</v>
       </c>
-      <c r="J1" s="27" t="s">
+      <c r="J1" s="24" t="s">
         <v>318</v>
       </c>
-      <c r="K1" s="27" t="s">
+      <c r="K1" s="24" t="s">
         <v>319</v>
       </c>
-      <c r="L1" s="27" t="s">
+      <c r="L1" s="24" t="s">
         <v>320</v>
       </c>
-      <c r="M1" s="27" t="s">
+      <c r="M1" s="24" t="s">
         <v>321</v>
       </c>
-      <c r="N1" s="27" t="s">
+      <c r="N1" s="24" t="s">
         <v>322</v>
       </c>
-      <c r="O1" s="27" t="s">
+      <c r="O1" s="24" t="s">
         <v>323</v>
       </c>
     </row>
@@ -6090,43 +6049,43 @@
       <c r="B2" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="C2" s="30">
+      <c r="C2" s="27">
         <v>45231</v>
       </c>
-      <c r="D2" s="31">
+      <c r="D2" s="28">
         <v>24505</v>
       </c>
-      <c r="E2" s="31" t="s">
+      <c r="E2" s="28" t="s">
         <v>325</v>
       </c>
-      <c r="F2" s="32">
+      <c r="F2" s="29">
         <v>106436</v>
       </c>
-      <c r="G2" s="32">
+      <c r="G2" s="29">
         <v>13550</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="I2" s="33" t="s">
+      <c r="I2" s="30" t="s">
         <v>327</v>
       </c>
-      <c r="J2" s="34" t="s">
+      <c r="J2" s="31" t="s">
         <v>328</v>
       </c>
-      <c r="K2" s="34" t="s">
+      <c r="K2" s="31" t="s">
         <v>328</v>
       </c>
-      <c r="L2" s="34" t="s">
+      <c r="L2" s="31" t="s">
         <v>328</v>
       </c>
-      <c r="M2" s="34" t="s">
+      <c r="M2" s="31" t="s">
         <v>328</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="O2" s="34" t="s">
+      <c r="O2" s="31" t="s">
         <v>328</v>
       </c>
     </row>
@@ -6157,25 +6116,24 @@
       <c r="B1" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="32" t="s">
         <v>330</v>
       </c>
-      <c r="E1" s="36">
-        <f>SUM(B2:B157)</f>
+      <c r="E1" s="33">
+        <v>15072</v>
+      </c>
+      <c r="F1" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="35" t="s">
+        <v>285</v>
+      </c>
+      <c r="B2" s="36">
         <v>1282</v>
       </c>
-      <c r="F1" s="37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
-        <v>285</v>
-      </c>
-      <c r="B2" s="39">
-        <v>1282</v>
-      </c>
-      <c r="C2" s="37">
+      <c r="C2" s="34">
         <v>8.4777145880174584E-2</v>
       </c>
     </row>

</xml_diff>